<commit_message>
added hydra and smartparens
</commit_message>
<xml_diff>
--- a/my_emacs_config.xlsx
+++ b/my_emacs_config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12330" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Org_Mode" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="408">
   <si>
     <t>Supporting Key</t>
   </si>
@@ -1234,6 +1234,18 @@
   </si>
   <si>
     <t>Insert \\qquad</t>
+  </si>
+  <si>
+    <t>Smartparens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projectile </t>
+  </si>
+  <si>
+    <t>Call with C-M-g (hydra)</t>
+  </si>
+  <si>
+    <t>Call with M-K (hydra)</t>
   </si>
 </sst>
 </file>
@@ -2649,10 +2661,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2990,6 +3002,14 @@
         <v>316</v>
       </c>
     </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>404</v>
+      </c>
+      <c r="B35" t="s">
+        <v>407</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2998,10 +3018,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3020,6 +3040,14 @@
       </c>
       <c r="B2" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -3371,7 +3399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added c-m-s for my-mark-sexp
</commit_message>
<xml_diff>
--- a/my_emacs_config.xlsx
+++ b/my_emacs_config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="410">
   <si>
     <t>Supporting Key</t>
   </si>
@@ -1246,6 +1246,12 @@
   </si>
   <si>
     <t>Call with M-K (hydra)</t>
+  </si>
+  <si>
+    <t>C-M-;</t>
+  </si>
+  <si>
+    <t>mark current variable or word</t>
   </si>
 </sst>
 </file>
@@ -2661,10 +2667,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3008,6 +3014,14 @@
       </c>
       <c r="B35" t="s">
         <v>407</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>408</v>
+      </c>
+      <c r="B37" t="s">
+        <v>409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
defined hydra for breadcrumb
</commit_message>
<xml_diff>
--- a/my_emacs_config.xlsx
+++ b/my_emacs_config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="412">
   <si>
     <t>Supporting Key</t>
   </si>
@@ -1252,6 +1252,12 @@
   </si>
   <si>
     <t>mark current variable or word</t>
+  </si>
+  <si>
+    <t>C-!</t>
+  </si>
+  <si>
+    <t>breadcrumb (hydra)</t>
   </si>
 </sst>
 </file>
@@ -2667,10 +2673,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3022,6 +3028,14 @@
       </c>
       <c r="B37" t="s">
         <v>409</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>410</v>
+      </c>
+      <c r="B38" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stop server;ace-window key change; added org hydra and zoom hydra
</commit_message>
<xml_diff>
--- a/my_emacs_config.xlsx
+++ b/my_emacs_config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Org_Mode" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Magit" sheetId="9" r:id="rId7"/>
     <sheet name="Evil" sheetId="10" r:id="rId8"/>
     <sheet name="cdlatex" sheetId="11" r:id="rId9"/>
+    <sheet name="appearance" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="418">
   <si>
     <t>Supporting Key</t>
   </si>
@@ -219,9 +220,6 @@
     <t>F8</t>
   </si>
   <si>
-    <t>insert sublevel item</t>
-  </si>
-  <si>
     <t>Narrow to Subtree</t>
   </si>
   <si>
@@ -597,9 +595,6 @@
     <t>bookmark-jump</t>
   </si>
   <si>
-    <t>M-L</t>
-  </si>
-  <si>
     <t>bookmark-bmenu-list</t>
   </si>
   <si>
@@ -1258,6 +1253,30 @@
   </si>
   <si>
     <t>breadcrumb (hydra)</t>
+  </si>
+  <si>
+    <t>M-F1</t>
+  </si>
+  <si>
+    <t>S-F1</t>
+  </si>
+  <si>
+    <t>breadcrumb hydra</t>
+  </si>
+  <si>
+    <t>C-M-!</t>
+  </si>
+  <si>
+    <t>M-a</t>
+  </si>
+  <si>
+    <t>C-M-z</t>
+  </si>
+  <si>
+    <t>zoom</t>
+  </si>
+  <si>
+    <t>org structural edit and move hydra</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1446,6 +1465,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1750,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1788,10 +1808,10 @@
         <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1812,10 +1832,10 @@
         <v>61</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1838,10 +1858,10 @@
         <v>62</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1862,10 +1882,10 @@
         <v>63</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1881,13 +1901,13 @@
         <v>64</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>65</v>
+        <v>417</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1905,13 +1925,13 @@
         <v>64</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1929,13 +1949,13 @@
         <v>64</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1948,16 +1968,16 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="J8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1970,16 +1990,16 @@
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="J9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1992,16 +2012,16 @@
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="J10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -2014,16 +2034,16 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="J11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -2036,16 +2056,16 @@
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="J12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -2058,16 +2078,16 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="J13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -2080,18 +2100,18 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -2104,42 +2124,42 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2152,18 +2172,18 @@
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>87</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
@@ -2178,18 +2198,18 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2204,18 +2224,18 @@
         <v>5</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2230,18 +2250,18 @@
         <v>7</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2254,18 +2274,18 @@
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2278,18 +2298,18 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2304,18 +2324,18 @@
         <v>6</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2330,18 +2350,18 @@
         <v>7</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2356,41 +2376,41 @@
         <v>5</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="K25" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="K25" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K26" s="11" t="s">
         <v>152</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2405,10 +2425,10 @@
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
       <c r="J27" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="K27" s="13" t="s">
         <v>182</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2437,10 +2457,10 @@
         <v>6</v>
       </c>
       <c r="F29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2454,10 +2474,10 @@
         <v>7</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -2465,129 +2485,129 @@
         <v>5</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E33" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="G33" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E34" s="8"/>
       <c r="F34" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E35" s="8"/>
       <c r="F35" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E36" s="8"/>
       <c r="F36" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E37" s="8"/>
       <c r="F37" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G37" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E38" s="8"/>
       <c r="F38" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="40" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E40" s="8"/>
       <c r="F40" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E42" s="8"/>
       <c r="F42" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="G42" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E44" s="8"/>
       <c r="F44" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E45" s="8"/>
       <c r="F45" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2596,12 +2616,35 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2612,58 +2655,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>315</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>413</v>
+      </c>
+      <c r="B12" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2675,8 +2726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2688,64 +2739,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>189</v>
-      </c>
       <c r="D1" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>3</v>
+        <v>410</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>191</v>
+        <v>411</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D4" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2753,103 +2804,103 @@
         <v>9</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D12" s="21" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D14" s="21" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2858,184 +2909,198 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D19" s="17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B20" s="23"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>304</v>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B35" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B37" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B38" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -3056,26 +3121,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -3099,24 +3164,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>184</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>186</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3206,58 +3271,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3277,10 +3342,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3300,122 +3365,122 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3435,354 +3500,354 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B12" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B17" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B18" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B19" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B20" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B21" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B22" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B23" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B24" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B25" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B26" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B29" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B30" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B32" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B33" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B34" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B35" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B36" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B38" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B39" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B40" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B41" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B42" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B43" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B44" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hydra for semantic and fa and hideshow
</commit_message>
<xml_diff>
--- a/my_emacs_config.xlsx
+++ b/my_emacs_config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12330"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12330" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Org_Mode" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="420">
   <si>
     <t>Supporting Key</t>
   </si>
@@ -1277,6 +1277,12 @@
   </si>
   <si>
     <t>org structural edit and move hydra</t>
+  </si>
+  <si>
+    <t>C-,</t>
+  </si>
+  <si>
+    <t>Hide Show</t>
   </si>
 </sst>
 </file>
@@ -1770,7 +1776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -2618,10 +2624,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2632,6 +2638,14 @@
       </c>
       <c r="B1" t="s">
         <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B3" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added emacs keys org file; unbind C-/ from undo tree
</commit_message>
<xml_diff>
--- a/my_emacs_config.xlsx
+++ b/my_emacs_config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12330" activeTab="10"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="24912" windowHeight="12276" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Org_Mode" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,16 @@
     <sheet name="cdlatex" sheetId="11" r:id="rId9"/>
     <sheet name="appearance" sheetId="12" r:id="rId10"/>
     <sheet name="Key-chord" sheetId="13" r:id="rId11"/>
+    <sheet name="ivy" sheetId="14" r:id="rId12"/>
+    <sheet name="helm" sheetId="15" r:id="rId13"/>
+    <sheet name="c_cpp" sheetId="16" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="460">
   <si>
     <t>Supporting Key</t>
   </si>
@@ -839,48 +842,21 @@
     <t>anzu-query-replace-regexp</t>
   </si>
   <si>
-    <t>C-c m</t>
-  </si>
-  <si>
-    <t>bc-set</t>
-  </si>
-  <si>
     <t>Breadcrumb</t>
   </si>
   <si>
-    <t>M-j</t>
-  </si>
-  <si>
     <t>bc-previous</t>
   </si>
   <si>
-    <t>S-M-j</t>
-  </si>
-  <si>
     <t>bc-next</t>
   </si>
   <si>
     <t>M-&lt;up&gt;</t>
   </si>
   <si>
-    <t>bc-local-previous</t>
-  </si>
-  <si>
     <t>M-&lt;down&gt;</t>
   </si>
   <si>
-    <t>bc-local-next</t>
-  </si>
-  <si>
-    <t>C-c C-l</t>
-  </si>
-  <si>
-    <t>bc-list</t>
-  </si>
-  <si>
-    <t>C-.</t>
-  </si>
-  <si>
     <t>C-&gt;</t>
   </si>
   <si>
@@ -1274,9 +1250,6 @@
     <t>C-M-z</t>
   </si>
   <si>
-    <t>zoom</t>
-  </si>
-  <si>
     <t>org structural edit and move hydra</t>
   </si>
   <si>
@@ -1298,10 +1271,142 @@
     <t>avy-goto-char-timer</t>
   </si>
   <si>
-    <t>sb</t>
-  </si>
-  <si>
     <t>helm-swoop-back-to-last-point</t>
+  </si>
+  <si>
+    <t>evaluate buffer</t>
+  </si>
+  <si>
+    <t>C-c I</t>
+  </si>
+  <si>
+    <t>load init file</t>
+  </si>
+  <si>
+    <t>c-c left</t>
+  </si>
+  <si>
+    <t>winner-undo</t>
+  </si>
+  <si>
+    <t>c-c right</t>
+  </si>
+  <si>
+    <t>winner-redo</t>
+  </si>
+  <si>
+    <t>ivy dired recent dirs</t>
+  </si>
+  <si>
+    <t>hydra-bm/body</t>
+  </si>
+  <si>
+    <t>M-F2</t>
+  </si>
+  <si>
+    <t>neotree toggle</t>
+  </si>
+  <si>
+    <t>ivy leading key</t>
+  </si>
+  <si>
+    <t>M-h</t>
+  </si>
+  <si>
+    <t>helm leading key</t>
+  </si>
+  <si>
+    <t>In helm map</t>
+  </si>
+  <si>
+    <t>helm follow action backward</t>
+  </si>
+  <si>
+    <t>helm follow action forward</t>
+  </si>
+  <si>
+    <t>ace helm line</t>
+  </si>
+  <si>
+    <t>swoop from isearch</t>
+  </si>
+  <si>
+    <t>M-h SPC</t>
+  </si>
+  <si>
+    <t>whack whitespace</t>
+  </si>
+  <si>
+    <t>avy goto char timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avy goto line </t>
+  </si>
+  <si>
+    <t>ww</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>keyboard quit</t>
+  </si>
+  <si>
+    <t>;;</t>
+  </si>
+  <si>
+    <t>end of line</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>beginning of line</t>
+  </si>
+  <si>
+    <t>zz</t>
+  </si>
+  <si>
+    <t>set mark command</t>
+  </si>
+  <si>
+    <t>zoom hydra</t>
+  </si>
+  <si>
+    <t>C-x \</t>
+  </si>
+  <si>
+    <t>indent buffer</t>
+  </si>
+  <si>
+    <t>c-c o</t>
+  </si>
+  <si>
+    <t>find other file in c</t>
+  </si>
+  <si>
+    <t>ff find other file</t>
+  </si>
+  <si>
+    <t>c- &gt;</t>
+  </si>
+  <si>
+    <t>highlight phrase</t>
+  </si>
+  <si>
+    <t>c-'</t>
+  </si>
+  <si>
+    <t>company complete common</t>
+  </si>
+  <si>
+    <t>flycheck previous error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-n </t>
+  </si>
+  <si>
+    <t>flycheck next error</t>
   </si>
 </sst>
 </file>
@@ -1799,23 +1904,23 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="1" max="1" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="12.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="2"/>
     <col min="10" max="10" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="76.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="11" max="11" width="76.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +1944,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -1863,7 +1968,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1889,7 +1994,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -1913,7 +2018,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +2031,7 @@
         <v>64</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>110</v>
@@ -1935,7 +2040,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1959,7 +2064,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>17</v>
@@ -1983,7 +2088,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>19</v>
@@ -2005,7 +2110,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>21</v>
@@ -2027,7 +2132,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>23</v>
@@ -2049,7 +2154,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>25</v>
@@ -2071,7 +2176,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>27</v>
@@ -2093,7 +2198,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>29</v>
@@ -2115,7 +2220,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>31</v>
@@ -2139,7 +2244,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>33</v>
@@ -2163,13 +2268,13 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
@@ -2187,7 +2292,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>34</v>
@@ -2211,7 +2316,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -2237,7 +2342,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>38</v>
@@ -2263,7 +2368,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>40</v>
@@ -2289,7 +2394,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>42</v>
@@ -2302,7 +2407,7 @@
         <v>92</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -2313,7 +2418,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>43</v>
@@ -2337,7 +2442,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
         <v>45</v>
@@ -2363,7 +2468,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>47</v>
@@ -2389,7 +2494,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>49</v>
@@ -2416,20 +2521,20 @@
       </c>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="11" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
         <v>99</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>151</v>
@@ -2438,7 +2543,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>51</v>
@@ -2456,7 +2561,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
@@ -2470,7 +2575,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>55</v>
@@ -2488,7 +2593,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>57</v>
       </c>
@@ -2505,7 +2610,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E31" s="4" t="s">
         <v>5</v>
       </c>
@@ -2516,7 +2621,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E33" s="8" t="s">
         <v>153</v>
       </c>
@@ -2527,7 +2632,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E34" s="8"/>
       <c r="F34" s="8" t="s">
         <v>156</v>
@@ -2536,7 +2641,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E35" s="8"/>
       <c r="F35" s="8" t="s">
         <v>158</v>
@@ -2545,7 +2650,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E36" s="8"/>
       <c r="F36" s="8" t="s">
         <v>160</v>
@@ -2554,7 +2659,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E37" s="8"/>
       <c r="F37" s="8" t="s">
         <v>162</v>
@@ -2563,7 +2668,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E38" s="8"/>
       <c r="F38" s="8" t="s">
         <v>164</v>
@@ -2572,7 +2677,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
         <v>166</v>
@@ -2581,7 +2686,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E40" s="8"/>
       <c r="F40" s="8" t="s">
         <v>168</v>
@@ -2590,7 +2695,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="41" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
         <v>170</v>
@@ -2599,7 +2704,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E42" s="8"/>
       <c r="F42" s="8" t="s">
         <v>172</v>
@@ -2608,7 +2713,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
         <v>174</v>
@@ -2617,7 +2722,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E44" s="8"/>
       <c r="F44" s="8" t="s">
         <v>176</v>
@@ -2626,7 +2731,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="E45" s="8"/>
       <c r="F45" s="8" t="s">
         <v>178</v>
@@ -2646,25 +2751,25 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="B1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="B3" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -2674,36 +2779,214 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B4" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>445</v>
+      </c>
+      <c r="B7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
         <v>422</v>
       </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>427</v>
+      </c>
       <c r="B1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" t="s">
+        <v>433</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>360</v>
+        <v>453</v>
       </c>
       <c r="B2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>424</v>
+        <v>455</v>
       </c>
       <c r="B3" t="s">
-        <v>425</v>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>458</v>
+      </c>
+      <c r="B5" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -2713,19 +2996,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>267</v>
       </c>
@@ -2733,7 +3016,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>269</v>
       </c>
@@ -2741,60 +3024,84 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="B7" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B12" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="B14" t="s">
-        <v>421</v>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>434</v>
+      </c>
+      <c r="B18" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>448</v>
+      </c>
+      <c r="B20" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -2804,383 +3111,389 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B2" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D2" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>410</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="E2" s="21"/>
+      <c r="G2" t="s">
+        <v>418</v>
+      </c>
+      <c r="H2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D3" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E3" s="21" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>411</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="G3" t="s">
+        <v>420</v>
+      </c>
+      <c r="H3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D4" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E4" s="21" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D4" s="21" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E5" s="21" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>424</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B8" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D8" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D8" s="21" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B11" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D11" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B12" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D12" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E12" s="21" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B13" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D13" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="21" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E14" s="21" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B15" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D15" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E15" s="21" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="21" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E16" s="21" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="B18" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E18" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="B19" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E19" s="21" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="B18" s="22" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" s="23"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="D23" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="D24" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="D25" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="D28" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="D30" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="E30" s="26" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D19" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B20" s="23"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
-        <v>271</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>291</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>274</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>275</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>293</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B31" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="D23" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
-        <v>278</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>279</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>297</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
-        <v>280</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>299</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
-        <v>282</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>414</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>94</v>
       </c>
-      <c r="B32" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>402</v>
-      </c>
-      <c r="B35" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="B37" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>408</v>
-      </c>
-      <c r="B38" t="s">
-        <v>409</v>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>397</v>
+      </c>
+      <c r="B39" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>399</v>
+      </c>
+      <c r="B40" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -3191,15 +3504,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>191</v>
       </c>
@@ -3207,7 +3520,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>198</v>
       </c>
@@ -3215,12 +3528,36 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="B4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>404</v>
+      </c>
+      <c r="B6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>450</v>
+      </c>
+      <c r="B9" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -3236,19 +3573,19 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>180</v>
       </c>
       <c r="B1" s="12"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>183</v>
       </c>
@@ -3256,7 +3593,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>185</v>
       </c>
@@ -3264,7 +3601,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -3273,7 +3610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -3282,7 +3619,7 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -3291,7 +3628,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
@@ -3300,7 +3637,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -3309,7 +3646,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -3320,7 +3657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -3344,60 +3681,60 @@
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" t="s">
         <v>291</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B6" t="s">
         <v>293</v>
       </c>
-      <c r="B2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>295</v>
-      </c>
-      <c r="B3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>299</v>
-      </c>
-      <c r="B5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>301</v>
-      </c>
-      <c r="B6" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -3418,9 +3755,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>200</v>
       </c>
@@ -3441,9 +3778,9 @@
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>244</v>
       </c>
@@ -3451,7 +3788,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>246</v>
       </c>
@@ -3459,7 +3796,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>248</v>
       </c>
@@ -3467,7 +3804,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>250</v>
       </c>
@@ -3475,7 +3812,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>252</v>
       </c>
@@ -3483,7 +3820,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>254</v>
       </c>
@@ -3491,7 +3828,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>255</v>
       </c>
@@ -3499,7 +3836,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>256</v>
       </c>
@@ -3507,7 +3844,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>258</v>
       </c>
@@ -3515,7 +3852,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>260</v>
       </c>
@@ -3523,7 +3860,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>261</v>
       </c>
@@ -3531,7 +3868,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>154</v>
       </c>
@@ -3539,7 +3876,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>263</v>
       </c>
@@ -3547,7 +3884,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>265</v>
       </c>
@@ -3555,7 +3892,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>266</v>
       </c>
@@ -3572,362 +3909,362 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection sqref="A1:B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>317</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B6" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>319</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>320</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>322</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>324</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>326</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>328</v>
       </c>
-      <c r="B7" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B12" t="s">
         <v>329</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B13" t="s">
         <v>331</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B14" t="s">
         <v>333</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>335</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>337</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B17" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>339</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B18" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>341</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B19" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>343</v>
       </c>
-      <c r="B15" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B20" t="s">
         <v>344</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B21" t="s">
         <v>346</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B22" t="s">
         <v>348</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B23" t="s">
         <v>350</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B24" t="s">
         <v>352</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B25" t="s">
         <v>354</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B26" t="s">
         <v>356</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B27" t="s">
         <v>358</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B28" t="s">
         <v>360</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B29" t="s">
         <v>362</v>
       </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B30" t="s">
         <v>364</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B31" t="s">
         <v>366</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B32" t="s">
         <v>368</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B33" t="s">
         <v>370</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B34" t="s">
         <v>372</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B35" t="s">
         <v>374</v>
       </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B36" t="s">
         <v>376</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B37" t="s">
         <v>378</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B38" t="s">
         <v>380</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B39" t="s">
         <v>382</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B40" t="s">
         <v>384</v>
       </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B41" t="s">
         <v>386</v>
       </c>
-      <c r="B37" t="s">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B42" t="s">
         <v>388</v>
       </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B43" t="s">
         <v>390</v>
       </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B44" t="s">
         <v>392</v>
-      </c>
-      <c r="B40" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>394</v>
-      </c>
-      <c r="B41" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>396</v>
-      </c>
-      <c r="B42" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>398</v>
-      </c>
-      <c r="B43" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>400</v>
-      </c>
-      <c r="B44" t="s">
-        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>